<commit_message>
Removed the cost table, unless provided from the finished contract document
</commit_message>
<xml_diff>
--- a/ContractApplikation/Data/TabelleKosten.xlsx
+++ b/ContractApplikation/Data/TabelleKosten.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t xml:space="preserve">Angebot </t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Std.</t>
-  </si>
-  <si>
-    <t>stundenpreis</t>
   </si>
   <si>
     <r>
@@ -76,9 +73,6 @@
     </r>
   </si>
   <si>
-    <t>preis</t>
-  </si>
-  <si>
     <t>Summe</t>
   </si>
 </sst>
@@ -86,19 +80,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -136,6 +124,25 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -212,55 +219,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,7 +588,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,16 +597,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -603,24 +625,24 @@
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="15"/>
+      <c r="G2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="14"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
@@ -633,53 +655,79 @@
       <c r="D4" s="6">
         <v>0</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="15"/>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="13">
+        <f>(D4*F4)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="A5" s="14">
+        <v>1.2</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="15">
+        <v>0</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0</v>
+      </c>
+      <c r="G5" s="13">
+        <f t="shared" ref="G5:G6" si="0">(D5*F5)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="A6" s="19">
+        <v>1.3</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="21">
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
-      <c r="B7" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13" t="s">
-        <v>10</v>
-      </c>
+      <c r="B7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="16">
+        <f>SUM(G4:H6)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B3:G3"/>
@@ -687,5 +735,6 @@
     <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added spire office dependency, included module in documentManager for adding table from excel sheet to the word document
</commit_message>
<xml_diff>
--- a/ContractApplikation/Data/TabelleKosten.xlsx
+++ b/ContractApplikation/Data/TabelleKosten.xlsx
@@ -219,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -248,41 +248,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,19 +590,18 @@
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+    <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -625,26 +618,24 @@
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="10"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -655,61 +646,55 @@
       <c r="D4" s="6">
         <v>0</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="6">
         <v>0</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="10">
         <f>(D4*F4)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
         <v>1.2</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="15">
-        <v>0</v>
-      </c>
-      <c r="E5" s="15" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="15">
-        <v>0</v>
-      </c>
-      <c r="G5" s="13">
-        <f t="shared" ref="G5:G6" si="0">(D5*F5)</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="13"/>
+      <c r="F5" s="11">
+        <v>0</v>
+      </c>
+      <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
         <v>1.3</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="21">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16">
         <v>0</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="21">
-        <v>0</v>
-      </c>
-      <c r="G6" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="13"/>
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
+        <f t="shared" ref="G6" si="0">(D6*F6)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="8" t="s">
         <v>8</v>
@@ -718,21 +703,15 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="16">
+      <c r="G7" s="8">
         <f>SUM(G4:H6)</f>
         <v>0</v>
       </c>
-      <c r="H7" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A1:H1"/>
+  <mergeCells count="2">
     <mergeCell ref="B3:G3"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>